<commit_message>
update on kerman nodes
</commit_message>
<xml_diff>
--- a/kerman/node_kerman.xlsx
+++ b/kerman/node_kerman.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\kerman\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\NetPlanner\kerman\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -101,76 +101,76 @@
     <t>AN</t>
   </si>
   <si>
-    <t>30.316080, 57.053855</t>
-  </si>
-  <si>
-    <t>30.316596, 57.073128</t>
-  </si>
-  <si>
-    <t>30.315851, 57.083149</t>
-  </si>
-  <si>
-    <t>30.311001, 57.057868</t>
-  </si>
-  <si>
-    <t>30.312043, 57.073891</t>
-  </si>
-  <si>
-    <t>30.308635, 57.086382</t>
-  </si>
-  <si>
-    <t>30.302451, 57.065282</t>
-  </si>
-  <si>
-    <t>30.298972, 57.074491</t>
-  </si>
-  <si>
-    <t>30.304315, 57.082341</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
-    <t>30.304394, 57.103931</t>
-  </si>
-  <si>
-    <t>30.291747, 57.113630</t>
-  </si>
-  <si>
-    <t>30.274597, 57.115527</t>
-  </si>
-  <si>
-    <t>30.261321, 57.102381</t>
-  </si>
-  <si>
-    <t>30.257864, 57.091987</t>
-  </si>
-  <si>
-    <t>30.279195, 57.082608</t>
-  </si>
-  <si>
-    <t>30.262729, 57.070752</t>
-  </si>
-  <si>
-    <t>30.284109, 57.067604</t>
-  </si>
-  <si>
-    <t>30.273707, 57.038340</t>
-  </si>
-  <si>
-    <t>30.302285, 57.026942</t>
-  </si>
-  <si>
-    <t>30.286598, 57.035542</t>
-  </si>
-  <si>
-    <t>30.294689, 57.022363</t>
-  </si>
-  <si>
-    <t>30.295381, 57.049223</t>
-  </si>
-  <si>
     <t>Directionless</t>
+  </si>
+  <si>
+    <t>30.311235, 57.033492</t>
+  </si>
+  <si>
+    <t>30.312610, 57.068984</t>
+  </si>
+  <si>
+    <t>30.307728, 57.098888</t>
+  </si>
+  <si>
+    <t>30.290032, 57.039864</t>
+  </si>
+  <si>
+    <t>30.292477, 57.089221</t>
+  </si>
+  <si>
+    <t>30.292568, 57.111453</t>
+  </si>
+  <si>
+    <t>30.264507, 57.049214</t>
+  </si>
+  <si>
+    <t>30.256178, 57.079154</t>
+  </si>
+  <si>
+    <t>30.262489, 57.106441</t>
+  </si>
+  <si>
+    <t>29.592670, 57.438840</t>
+  </si>
+  <si>
+    <t>29.100416, 58.369935</t>
+  </si>
+  <si>
+    <t>28.735959, 57.330483</t>
+  </si>
+  <si>
+    <t>28.163476, 57.312216</t>
+  </si>
+  <si>
+    <t>28.812881, 56.547009</t>
+  </si>
+  <si>
+    <t>29.858242, 56.798987</t>
+  </si>
+  <si>
+    <t>29.430221, 55.672557</t>
+  </si>
+  <si>
+    <t>29.927019, 56.567369</t>
+  </si>
+  <si>
+    <t>30.114571, 55.124759</t>
+  </si>
+  <si>
+    <t>29.998328, 55.791895</t>
+  </si>
+  <si>
+    <t>30.810333, 56.586627</t>
+  </si>
+  <si>
+    <t>30.886843, 55.243911</t>
+  </si>
+  <si>
+    <t>30.399309, 56.001607</t>
   </si>
 </sst>
 </file>
@@ -1703,7 +1703,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1736,10 +1736,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1750,10 +1750,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1764,10 +1764,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1778,10 +1778,10 @@
         <v>7</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1792,10 +1792,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1806,10 +1806,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1820,10 +1820,10 @@
         <v>10</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1834,10 +1834,10 @@
         <v>11</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1848,10 +1848,10 @@
         <v>12</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1859,13 +1859,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1876,10 +1876,10 @@
         <v>13</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1890,10 +1890,10 @@
         <v>14</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1904,10 +1904,10 @@
         <v>15</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1918,10 +1918,10 @@
         <v>16</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1932,10 +1932,10 @@
         <v>17</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1946,10 +1946,10 @@
         <v>18</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1960,10 +1960,10 @@
         <v>19</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1974,10 +1974,10 @@
         <v>20</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1991,7 +1991,7 @@
         <v>45</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2002,10 +2002,10 @@
         <v>22</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2016,10 +2016,10 @@
         <v>23</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2030,13 +2030,14 @@
         <v>24</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>